<commit_message>
Update LO and Key mapping logic to support new 9-column Excel format
</commit_message>
<xml_diff>
--- a/SCERT 1.xlsx
+++ b/SCERT 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Viswam Report card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089D6ED6-B33E-42C5-B46D-BBCBE368CDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E57568B-E042-43D7-831D-149A873CF496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
   <si>
     <t>M1</t>
   </si>
@@ -172,13 +172,142 @@
   </si>
   <si>
     <t>E15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject </t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Lo</t>
+  </si>
+  <si>
+    <t>Use of percent</t>
+  </si>
+  <si>
+    <t>Division of decimal numbers</t>
+  </si>
+  <si>
+    <t>Two special Triangles : Equilateral and Isosceles</t>
+  </si>
+  <si>
+    <t>Properties of addition and subtraction of Integers</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Application of simple equation to practical situations</t>
+  </si>
+  <si>
+    <t>Pairs of Lines</t>
+  </si>
+  <si>
+    <t>Operation on rational number</t>
+  </si>
+  <si>
+    <t>Sum of the length of two sides of a triangle</t>
+  </si>
+  <si>
+    <t>Circle graph or pie chart</t>
+  </si>
+  <si>
+    <t>Setting up of an equation</t>
+  </si>
+  <si>
+    <t>Checking for parallel lines</t>
+  </si>
+  <si>
+    <t>What do various nutrients do for our body</t>
+  </si>
+  <si>
+    <t>Acids and Bases</t>
+  </si>
+  <si>
+    <t>Silk</t>
+  </si>
+  <si>
+    <t>Measuring speed</t>
+  </si>
+  <si>
+    <t>Measuring temperature</t>
+  </si>
+  <si>
+    <t>Climate</t>
+  </si>
+  <si>
+    <t>Heating effect of electric current</t>
+  </si>
+  <si>
+    <t>wind currents are generated due to uneven heating on the earth</t>
+  </si>
+  <si>
+    <t>Hot and cold</t>
+  </si>
+  <si>
+    <t>Reflection of Light</t>
+  </si>
+  <si>
+    <t>Photosynthesis - food making process in plants</t>
+  </si>
+  <si>
+    <t>Why do we Respire</t>
+  </si>
+  <si>
+    <t>Mode of Reproduction</t>
+  </si>
+  <si>
+    <t>Seed Dispersal</t>
+  </si>
+  <si>
+    <t>Climate and adaptation</t>
+  </si>
+  <si>
+    <t>Retrieve and record information/identify key details from fiction and non-fiction.</t>
+  </si>
+  <si>
+    <t>Identify/explain how meaning is enhanced through choice of words and phrases.</t>
+  </si>
+  <si>
+    <t>Identify/explain how information/narrative content is related and contributes to meanings as a whole.</t>
+  </si>
+  <si>
+    <t>Comprehend literal information.</t>
+  </si>
+  <si>
+    <t>Predict what might happen from details stated and implied.</t>
+  </si>
+  <si>
+    <t>Verb</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Preposition</t>
+  </si>
+  <si>
+    <t>Punctuation</t>
+  </si>
+  <si>
+    <t>Synonym</t>
+  </si>
+  <si>
+    <t>Summarise main ideas from more than one paragraph.</t>
+  </si>
+  <si>
+    <t>Make inferences from the text/explain and justify inferences with evidence from the text.</t>
+  </si>
+  <si>
+    <t>Make comparisons within the text.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,16 +327,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -230,15 +379,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,312 +714,479 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="7" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
+      <c r="I6" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
+      <c r="H7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="1" t="s">
+      <c r="H10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
+      <c r="I12" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="1" t="s">
+      <c r="H13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="1" t="s">
+      <c r="H14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="1" t="s">
+      <c r="H15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>10</v>
+      <c r="H16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>